<commit_message>
Remove bugs from PLOS Revised version
 * Add onOtherDataSet = True to binary encoding
 * Fix correct_consecutive = 2 coherently
</commit_message>
<xml_diff>
--- a/figures/fig2/fig2B.xlsx
+++ b/figures/fig2/fig2B.xlsx
@@ -441,7 +441,7 @@
         <v>6.016666666666667</v>
       </c>
       <c r="E2">
-        <v>4.889545207316344</v>
+        <v>3.36737340994749</v>
       </c>
       <c r="F2">
         <v>19.96001767744599</v>
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>8.847646729259548</v>
+        <v>9.452302473339424</v>
       </c>
       <c r="I2">
-        <v>6.228583738355953</v>
+        <v>7.146166390990507</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -470,7 +470,7 @@
         <v>10.02777777777778</v>
       </c>
       <c r="E3">
-        <v>4.626238300122376</v>
+        <v>4.204847452378137</v>
       </c>
       <c r="F3">
         <v>11.97601060646759</v>
@@ -479,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>5.42174813607379</v>
+        <v>5.684591802882636</v>
       </c>
       <c r="I3">
-        <v>1.933096476247085</v>
+        <v>2.09143060934584</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -499,7 +499,7 @@
         <v>14.03888888888889</v>
       </c>
       <c r="E4">
-        <v>4.168932857081169</v>
+        <v>3.957198220786172</v>
       </c>
       <c r="F4">
         <v>8.554293290333996</v>
@@ -508,10 +508,10 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>3.281064451400041</v>
+        <v>3.473176571249101</v>
       </c>
       <c r="I4">
-        <v>1.107526583905577</v>
+        <v>1.126633137245187</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -528,7 +528,7 @@
         <v>20.03994688015306</v>
       </c>
       <c r="E5">
-        <v>3.583117853359836</v>
+        <v>3.37502721062112</v>
       </c>
       <c r="F5">
         <v>5.988305484922114</v>
@@ -537,10 +537,10 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1.850831279969574</v>
+        <v>2.025145410352073</v>
       </c>
       <c r="I5">
-        <v>0.5579560049167881</v>
+        <v>0.5911471402326958</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -557,7 +557,7 @@
         <v>30.05946714266826</v>
       </c>
       <c r="E6">
-        <v>2.688268610539874</v>
+        <v>2.63891650368598</v>
       </c>
       <c r="F6">
         <v>3.992207273194541</v>
@@ -566,10 +566,10 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1.059553260017393</v>
+        <v>1.101808447138428</v>
       </c>
       <c r="I6">
-        <v>0.247919244033429</v>
+        <v>0.2544740607618841</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -586,7 +586,7 @@
         <v>40.03623154438466</v>
       </c>
       <c r="E7">
-        <v>2.201709104861691</v>
+        <v>2.114078642529698</v>
       </c>
       <c r="F7">
         <v>2.994266036207903</v>
@@ -595,10 +595,10 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0.5623681922938342</v>
+        <v>0.6433867657716956</v>
       </c>
       <c r="I7">
-        <v>0.2324247139757737</v>
+        <v>0.2386662659489538</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -615,7 +615,7 @@
         <v>60.24926509446954</v>
       </c>
       <c r="E8">
-        <v>1.543375415602326</v>
+        <v>1.466625761326899</v>
       </c>
       <c r="F8">
         <v>1.995744018324527</v>
@@ -624,10 +624,10 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.3273264879377785</v>
+        <v>0.4102779839055163</v>
       </c>
       <c r="I8">
-        <v>0.1261305104230151</v>
+        <v>0.1197929858967771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>